<commit_message>
added jesse again to the docs and excel
</commit_message>
<xml_diff>
--- a/Requirements_Traceability_Matrix.xlsx
+++ b/Requirements_Traceability_Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hamad Ahmed\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blloyd\Documents\P_Projects\Vox_Design_Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1A11EA-EDBC-4C7A-B3DC-C2BE8247CE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3F455A-2DC6-4010-A3E9-D48617EFFA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1 SRS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
   <si>
     <t>SRS Section ID</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>3.8.2</t>
+  </si>
+  <si>
+    <t>Jesse</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -606,10 +609,10 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.88671875" customWidth="1"/>
@@ -617,7 +620,7 @@
     <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,7 +651,7 @@
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4">
         <v>3.1</v>
       </c>
@@ -665,7 +668,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4">
         <v>3.2</v>
       </c>
@@ -682,7 +685,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4">
         <v>3.3</v>
       </c>
@@ -699,7 +702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>3.4</v>
       </c>
@@ -707,7 +710,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>42</v>
@@ -716,7 +719,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>3.5</v>
       </c>
@@ -733,7 +736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4">
         <v>3.6</v>
       </c>
@@ -750,7 +753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>3.7</v>
       </c>
@@ -767,7 +770,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
         <v>43</v>
       </c>
@@ -784,7 +787,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>44</v>
       </c>
@@ -801,7 +804,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4">
         <v>3.9</v>
       </c>
@@ -809,7 +812,7 @@
         <v>33</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>42</v>
@@ -818,7 +821,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="9">
         <v>3.1</v>
       </c>
@@ -835,7 +838,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4">
         <v>3.11</v>
       </c>
@@ -852,7 +855,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4">
         <v>3.12</v>
       </c>
@@ -892,9 +895,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -935,12 +938,12 @@
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4">
         <v>3.2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="str">
         <f>HYPERLINK("https://docs.google.com/document/d/1SjNQH7gAA9u9Y_R3xWQgdJfR8mdQ7Ad-hjht9vqAj9w/edit#heading=h.uf9m6nfmmef3","3.2.1")</f>
         <v>3.2.1</v>
@@ -949,13 +952,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="str">
         <f>HYPERLINK("https://docs.google.com/document/d/1SjNQH7gAA9u9Y_R3xWQgdJfR8mdQ7Ad-hjht9vqAj9w/edit#heading=h.ug5g3rb1dlsm","3.2.2")</f>
         <v>3.2.2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="str">
         <f>HYPERLINK("https://docs.google.com/document/d/1SjNQH7gAA9u9Y_R3xWQgdJfR8mdQ7Ad-hjht9vqAj9w/edit#heading=h.cfr3r3i641kp","3.2.3")</f>
         <v>3.2.3</v>
@@ -983,9 +986,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1051,13 +1054,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.44140625" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1119,7 @@
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
     </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="str">
         <f>HYPERLINK("https://docs.google.com/document/d/1SjNQH7gAA9u9Y_R3xWQgdJfR8mdQ7Ad-hjht9vqAj9w/edit#heading=h.uf9m6nfmmef3","3.2.1")</f>
         <v>3.2.1</v>
@@ -1128,7 +1131,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J6" s="4">
         <v>1</v>
       </c>
@@ -1139,7 +1142,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J7" s="4">
         <v>2</v>
       </c>
@@ -1150,7 +1153,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="J8" s="4">
         <v>3</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>

</xml_diff>